<commit_message>
Edited readme, added neural network
</commit_message>
<xml_diff>
--- a/moran-strategies-scores.xlsx
+++ b/moran-strategies-scores.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Players" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>max</t>
   </si>
@@ -98,6 +97,9 @@
   </si>
   <si>
     <t>Size algorith: max degree node of the largest player</t>
+  </si>
+  <si>
+    <t>min+drop smallest</t>
   </si>
 </sst>
 </file>
@@ -157,10 +159,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -168,7 +170,558 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -444,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:P19"/>
+  <dimension ref="C2:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,35 +1010,35 @@
     <col min="16" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D2" s="4" t="s">
+    <row r="2" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D3" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="O3" s="5" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="Q3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>7</v>
       </c>
@@ -516,20 +1069,23 @@
       <c r="L4">
         <v>3000</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -560,24 +1116,27 @@
       <c r="L5">
         <v>9150</v>
       </c>
-      <c r="M5" s="3">
-        <f>AVERAGE(D5:L5)</f>
-        <v>7712.7777777777774</v>
-      </c>
-      <c r="N5" s="2">
-        <f>_xlfn.STDEV.P(D5:L5)/M5</f>
-        <v>0.17033350890390575</v>
+      <c r="M5">
+        <v>6214</v>
       </c>
       <c r="O5" s="3">
-        <f>M5*(1-2*N5/SQRT(COUNT(D5:L5)))</f>
-        <v>6836.9481095878064</v>
-      </c>
-      <c r="P5" s="3">
-        <f>M5*(1+2*N5/SQRT(COUNT(D5:L5)))</f>
-        <v>8588.6074459677493</v>
-      </c>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+        <f>AVERAGE(D5:M5)</f>
+        <v>7562.9</v>
+      </c>
+      <c r="P5" s="2">
+        <f>_xlfn.STDEV.P(D5:M5)/O5</f>
+        <v>0.17519122208814833</v>
+      </c>
+      <c r="Q5" s="3">
+        <f>O5*(1-2*P5/SQRT(COUNT(D5:M5)))</f>
+        <v>6724.9257068382103</v>
+      </c>
+      <c r="R5" s="3">
+        <f>O5*(1+2*P5/SQRT(COUNT(D5:M5)))</f>
+        <v>8400.874293161789</v>
+      </c>
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -608,24 +1167,27 @@
       <c r="L6">
         <v>8871</v>
       </c>
-      <c r="M6" s="3">
-        <f>AVERAGE(D6:L6)</f>
-        <v>8021.7777777777774</v>
-      </c>
-      <c r="N6" s="2">
-        <f>_xlfn.STDEV.P(D6:L6)/M6</f>
-        <v>0.19470224432449584</v>
+      <c r="M6">
+        <v>7494</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" ref="O6:O9" si="0">M6*(1-2*N6/SQRT(COUNT(D6:L6)))</f>
-        <v>6980.5390199073108</v>
-      </c>
-      <c r="P6" s="3">
-        <f t="shared" ref="P6:P9" si="1">M6*(1+2*N6/SQRT(COUNT(D6:L6)))</f>
-        <v>9063.016535648243</v>
-      </c>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+        <f t="shared" ref="O6:O10" si="0">AVERAGE(D6:M6)</f>
+        <v>7969</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" ref="P6:P10" si="1">_xlfn.STDEV.P(D6:M6)/O6</f>
+        <v>0.18699264091144766</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" ref="Q6:Q10" si="2">O6*(1-2*P6/SQRT(COUNT(D6:M6)))</f>
+        <v>7026.5499588837611</v>
+      </c>
+      <c r="R6" s="3">
+        <f t="shared" ref="R6:R10" si="3">O6*(1+2*P6/SQRT(COUNT(D6:M6)))</f>
+        <v>8911.4500411162389</v>
+      </c>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>2</v>
       </c>
@@ -656,24 +1218,27 @@
       <c r="L7">
         <v>9281</v>
       </c>
-      <c r="M7" s="3">
-        <f>AVERAGE(D7:L7)</f>
-        <v>8330.5555555555547</v>
-      </c>
-      <c r="N7" s="2">
-        <f>_xlfn.STDEV.P(D7:L7)/M7</f>
-        <v>0.17180877484136572</v>
+      <c r="M7">
+        <v>7492</v>
       </c>
       <c r="O7" s="3">
-        <f>M7*(1-2*N7/SQRT(COUNT(D7:L7)))</f>
-        <v>7376.3805263902659</v>
-      </c>
-      <c r="P7" s="3">
+        <f t="shared" si="0"/>
+        <v>8246.7000000000007</v>
+      </c>
+      <c r="P7" s="2">
         <f t="shared" si="1"/>
-        <v>9284.7305847208427</v>
-      </c>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+        <v>0.16745152865513091</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="2"/>
+        <v>7373.3279120558072</v>
+      </c>
+      <c r="R7" s="3">
+        <f t="shared" si="3"/>
+        <v>9120.0720879441942</v>
+      </c>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>13</v>
       </c>
@@ -704,24 +1269,27 @@
       <c r="L8">
         <v>9585</v>
       </c>
-      <c r="M8" s="3">
-        <f t="shared" ref="M8:M9" si="2">AVERAGE(D8:L8)</f>
-        <v>7944.666666666667</v>
-      </c>
-      <c r="N8" s="2">
-        <f t="shared" ref="N8:N9" si="3">_xlfn.STDEV.P(D8:L8)/M8</f>
-        <v>0.14993372464184657</v>
+      <c r="M8">
+        <v>7774</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="0"/>
-        <v>7150.551023752495</v>
-      </c>
-      <c r="P8" s="3">
+        <v>7927.6</v>
+      </c>
+      <c r="P8" s="2">
         <f t="shared" si="1"/>
-        <v>8738.782309580838</v>
-      </c>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+        <v>0.14269207044937679</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="2"/>
+        <v>7212.1627239233339</v>
+      </c>
+      <c r="R8" s="3">
+        <f t="shared" si="3"/>
+        <v>8643.0372760766677</v>
+      </c>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>14</v>
       </c>
@@ -752,24 +1320,27 @@
       <c r="L9">
         <v>8363</v>
       </c>
-      <c r="M9" s="3">
-        <f t="shared" si="2"/>
-        <v>7580.4444444444443</v>
-      </c>
-      <c r="N9" s="2">
-        <f t="shared" si="3"/>
-        <v>8.8180599856194239E-2</v>
+      <c r="M9">
+        <v>6492</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="0"/>
-        <v>7134.8123522526666</v>
-      </c>
-      <c r="P9" s="3">
+        <v>7471.6</v>
+      </c>
+      <c r="P9" s="2">
         <f t="shared" si="1"/>
-        <v>8026.076536636222</v>
-      </c>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+        <v>9.5465147149902965E-2</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" si="2"/>
+        <v>7020.4837666410131</v>
+      </c>
+      <c r="R9" s="3">
+        <f t="shared" si="3"/>
+        <v>7922.7162333589868</v>
+      </c>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>15</v>
       </c>
@@ -800,246 +1371,346 @@
       <c r="L10">
         <v>9538</v>
       </c>
-      <c r="M10" s="3">
-        <f t="shared" ref="M10" si="4">AVERAGE(D10:L10)</f>
-        <v>8149</v>
-      </c>
-      <c r="N10" s="2">
-        <f>_xlfn.STDEV.P(D10:L10)/M10</f>
-        <v>0.1752931142463045</v>
+      <c r="M10">
+        <v>8626</v>
       </c>
       <c r="O10" s="3">
-        <f t="shared" ref="O10" si="5">M10*(1-2*N10/SQRT(COUNT(D10:L10)))</f>
-        <v>7196.6909413379099</v>
-      </c>
-      <c r="P10" s="3">
-        <f t="shared" ref="P10" si="6">M10*(1+2*N10/SQRT(COUNT(D10:L10)))</f>
-        <v>9101.3090586620892</v>
-      </c>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D11" s="4" t="s">
+        <f t="shared" si="0"/>
+        <v>8196.7000000000007</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16624910348699054</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" si="2"/>
+        <v>7334.85662443806</v>
+      </c>
+      <c r="R10" s="3">
+        <f t="shared" si="3"/>
+        <v>9058.5433755619415</v>
+      </c>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>6188</v>
+      </c>
+      <c r="E11">
+        <v>7739</v>
+      </c>
+      <c r="F11">
+        <v>9088</v>
+      </c>
+      <c r="G11">
+        <v>8622</v>
+      </c>
+      <c r="H11">
+        <v>6781</v>
+      </c>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D12" s="4" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>7</v>
       </c>
-      <c r="D13">
+      <c r="D17">
         <v>42</v>
       </c>
-      <c r="E13">
+      <c r="E17">
         <v>33</v>
       </c>
-      <c r="F13">
+      <c r="F17">
         <v>123</v>
       </c>
-      <c r="G13">
+      <c r="G17">
         <v>1234</v>
       </c>
-      <c r="H13">
+      <c r="H17">
         <v>8</v>
       </c>
-      <c r="I13">
+      <c r="I17">
         <v>2022</v>
       </c>
-      <c r="J13">
+      <c r="J17">
         <v>27</v>
       </c>
-      <c r="K13">
+      <c r="K17">
         <v>2000</v>
       </c>
-      <c r="L13">
+      <c r="L17">
         <v>3000</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14" s="1">
-        <f>SUM(D14:L14)</f>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <f>SUM(D18:M18)</f>
         <v>3</v>
       </c>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15" s="1">
-        <f t="shared" ref="M15:M19" si="7">SUM(D15:L15)</f>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" ref="O19:O23" si="4">SUM(D19:M19)</f>
         <v>5</v>
       </c>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16" s="1">
-        <f t="shared" si="7"/>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>13</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17" s="1">
-        <f t="shared" si="7"/>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>14</v>
       </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18" s="1">
-        <f t="shared" si="7"/>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>15</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19" s="1">
-        <f t="shared" si="7"/>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="D2:K2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="D15:K15"/>
     <mergeCell ref="D3:K3"/>
   </mergeCells>
+  <conditionalFormatting sqref="O5:O10">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+      <formula>MAX($O$5:$O$10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+      <formula>MIN($O$5:$O$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5:P10">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+      <formula>MIN($P$5:$P$10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+      <formula>MAX($P$5:$P$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5:Q10">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>MAX($Q$5:$Q$10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+      <formula>MIN($Q$5:$Q$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5:R10">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>MAX($R$5:$R$10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+      <formula>MIN($R$5:$R$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O18:O23">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+      <formula>MAX($O$18:$O$23)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>MIN($O$18:$O$23)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel file updates and removed model summary output
</commit_message>
<xml_diff>
--- a/moran-strategies-scores.xlsx
+++ b/moran-strategies-scores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="36">
   <si>
     <t xml:space="preserve">Score</t>
   </si>
@@ -115,16 +115,22 @@
     <t xml:space="preserve">CI95-high</t>
   </si>
   <si>
+    <t xml:space="preserve">seed:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4in-123nn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4in-13nn</t>
+  </si>
+  <si>
     <t xml:space="preserve">won</t>
-  </si>
-  <si>
-    <t xml:space="preserve">score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4in-123nn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4in-13nn</t>
   </si>
 </sst>
 </file>
@@ -214,7 +220,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -252,6 +258,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,8 +446,8 @@
   </sheetPr>
   <dimension ref="C2:R34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O17" activeCellId="0" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1764,64 +1774,362 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C1:E5"/>
+  <dimension ref="C1:R18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="0" t="n">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>31</v>
-      </c>
+      <c r="F2" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="D4" s="0" t="n">
+        <v>6997</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>9651</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>8038</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="n">
+        <v>9377</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>9769</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>6088</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>9144</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>8593</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>6075</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>9281</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>7492</v>
+      </c>
+      <c r="O4" s="4" t="n">
+        <f aca="false">AVERAGE(D4:M4)</f>
+        <v>8246.7</v>
+      </c>
+      <c r="P4" s="5" t="n">
+        <f aca="false">_xlfn.STDEV.P(D4:M4)/O4</f>
+        <v>0.167451528655131</v>
+      </c>
+      <c r="Q4" s="4" t="n">
+        <f aca="false">O4*(1-2*P4/SQRT(COUNT(D4:M4)))</f>
+        <v>7373.32791205581</v>
+      </c>
+      <c r="R4" s="4" t="n">
+        <f aca="false">O4*(1+2*P4/SQRT(COUNT(D4:M4)))</f>
+        <v>9120.07208794419</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="E5" s="0" t="n">
+        <v>8038</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <f aca="false">AVERAGE(D5:M5)</f>
+        <v>8038</v>
+      </c>
+      <c r="P5" s="5" t="n">
+        <f aca="false">_xlfn.STDEV.P(D5:M5)/O5</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4" t="n">
+        <f aca="false">O5*(1-2*P5/SQRT(COUNT(D5:M5)))</f>
+        <v>8038</v>
+      </c>
+      <c r="R5" s="4" t="n">
+        <f aca="false">O5*(1+2*P5/SQRT(COUNT(D5:M5)))</f>
+        <v>8038</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>8766</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>9609</v>
       </c>
-    </row>
+      <c r="O6" s="4" t="n">
+        <f aca="false">AVERAGE(D6:M6)</f>
+        <v>9187.5</v>
+      </c>
+      <c r="P6" s="5" t="n">
+        <f aca="false">_xlfn.STDEV.P(D6:M6)/O6</f>
+        <v>0.0458775510204082</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <f aca="false">O6*(1-2*P6/SQRT(COUNT(D6:M6)))</f>
+        <v>8591.40898345974</v>
+      </c>
+      <c r="R6" s="4" t="n">
+        <f aca="false">O6*(1+2*P6/SQRT(COUNT(D6:M6)))</f>
+        <v>9783.59101654026</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="6" t="n">
+        <f aca="false">SUM(D11:M11)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="6" t="n">
+        <f aca="false">SUM(D12:M12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="6" t="n">
+        <f aca="false">SUM(D13:M13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Q2:R2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="O4:O6">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>MIN($O$5:$O$10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>MAX($O$5:$O$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:P6">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>MAX($P$5:$P$10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>MIN($P$5:$P$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4:Q6">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>MIN($Q$5:$Q$10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+      <formula>MAX($Q$5:$Q$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:R6">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+      <formula>MIN($R$5:$R$10)</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>MAX($R$5:$R$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O11:O13">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>MIN($O$18:$O$23)</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+      <formula>MAX($O$18:$O$23)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added static seed to nn
</commit_message>
<xml_diff>
--- a/moran-strategies-scores.xlsx
+++ b/moran-strategies-scores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
   <si>
     <t xml:space="preserve">Score</t>
   </si>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Omada52</t>
   </si>
   <si>
-    <t xml:space="preserve">Size algorith: max degree node of the largest player</t>
+    <t xml:space="preserve">Size algorithm: max degree node of the largest player</t>
   </si>
   <si>
     <t xml:space="preserve">Omada53</t>
@@ -103,9 +103,6 @@
     <t xml:space="preserve">Revenge algorithm: min degree node of player with the highest attack count </t>
   </si>
   <si>
-    <t xml:space="preserve">Size algorithm: max degree node of the largest player</t>
-  </si>
-  <si>
     <t xml:space="preserve">seed from 0-1000, 1 game per seed</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">won</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neural Network</t>
   </si>
 </sst>
 </file>
@@ -220,7 +220,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -261,7 +261,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -446,8 +450,8 @@
   </sheetPr>
   <dimension ref="C2:R34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O17" activeCellId="0" sqref="O17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P10" activeCellId="0" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1598,7 +1602,7 @@
         <v>21</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,7 +1683,7 @@
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.15"/>
@@ -1694,7 +1698,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1708,10 +1712,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>16</v>
@@ -1774,18 +1778,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C1:R18"/>
+  <dimension ref="C1:R30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>42</v>
@@ -1824,37 +1828,37 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="E3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>4</v>
@@ -1869,7 +1873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
         <v>10</v>
       </c>
@@ -1903,50 +1907,77 @@
       <c r="M4" s="0" t="n">
         <v>7492</v>
       </c>
-      <c r="O4" s="4" t="n">
+      <c r="O4" s="10" t="n">
         <f aca="false">AVERAGE(D4:M4)</f>
         <v>8246.7</v>
       </c>
-      <c r="P4" s="5" t="n">
+      <c r="P4" s="11" t="n">
         <f aca="false">_xlfn.STDEV.P(D4:M4)/O4</f>
         <v>0.167451528655131</v>
       </c>
-      <c r="Q4" s="4" t="n">
+      <c r="Q4" s="10" t="n">
         <f aca="false">O4*(1-2*P4/SQRT(COUNT(D4:M4)))</f>
         <v>7373.32791205581</v>
       </c>
-      <c r="R4" s="4" t="n">
+      <c r="R4" s="10" t="n">
         <f aca="false">O4*(1+2*P4/SQRT(COUNT(D4:M4)))</f>
         <v>9120.07208794419</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7664</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>8038</v>
       </c>
-      <c r="O5" s="4" t="n">
+      <c r="F5" s="0" t="n">
+        <v>7706</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>10171</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>5372</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>8763</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>7213</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>7532</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>9310</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>6998</v>
+      </c>
+      <c r="O5" s="10" t="n">
         <f aca="false">AVERAGE(D5:M5)</f>
-        <v>8038</v>
-      </c>
-      <c r="P5" s="5" t="n">
+        <v>7876.7</v>
+      </c>
+      <c r="P5" s="11" t="n">
         <f aca="false">_xlfn.STDEV.P(D5:M5)/O5</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4" t="n">
+        <v>0.159627759583732</v>
+      </c>
+      <c r="Q5" s="10" t="n">
         <f aca="false">O5*(1-2*P5/SQRT(COUNT(D5:M5)))</f>
-        <v>8038</v>
-      </c>
-      <c r="R5" s="4" t="n">
+        <v>7081.48837785153</v>
+      </c>
+      <c r="R5" s="10" t="n">
         <f aca="false">O5*(1+2*P5/SQRT(COUNT(D5:M5)))</f>
-        <v>8038</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8671.91162214847</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>8766</v>
@@ -1954,62 +1985,86 @@
       <c r="E6" s="0" t="n">
         <v>9609</v>
       </c>
-      <c r="O6" s="4" t="n">
+      <c r="F6" s="0" t="n">
+        <v>7510</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>9271</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>6216</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>7686</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>8102</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>7756</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>9152</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>6323</v>
+      </c>
+      <c r="O6" s="10" t="n">
         <f aca="false">AVERAGE(D6:M6)</f>
-        <v>9187.5</v>
-      </c>
-      <c r="P6" s="5" t="n">
+        <v>8039.1</v>
+      </c>
+      <c r="P6" s="11" t="n">
         <f aca="false">_xlfn.STDEV.P(D6:M6)/O6</f>
-        <v>0.0458775510204082</v>
-      </c>
-      <c r="Q6" s="4" t="n">
+        <v>0.139110759411143</v>
+      </c>
+      <c r="Q6" s="10" t="n">
         <f aca="false">O6*(1-2*P6/SQRT(COUNT(D6:M6)))</f>
-        <v>8591.40898345974</v>
-      </c>
-      <c r="R6" s="4" t="n">
+        <v>7331.80897361836</v>
+      </c>
+      <c r="R6" s="10" t="n">
         <f aca="false">O6*(1+2*P6/SQRT(COUNT(D6:M6)))</f>
-        <v>9783.59101654026</v>
+        <v>8746.39102638164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P7" s="10"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P8" s="10"/>
+      <c r="P8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P9" s="10"/>
+      <c r="P9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>16</v>
@@ -2056,29 +2111,80 @@
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O12" s="6" t="n">
         <f aca="false">SUM(D12:M12)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="O13" s="6" t="n">
         <f aca="false">SUM(D13:M13)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2086,47 +2192,47 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="Q2:R2"/>
   </mergeCells>
-  <conditionalFormatting sqref="O4:O6">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>MIN($O$5:$O$10)</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>MAX($O$5:$O$10)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P6">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>MAX($P$5:$P$10)</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>MIN($P$5:$P$10)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q4:Q6">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>MIN($Q$5:$Q$10)</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>MAX($Q$5:$Q$10)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R4:R6">
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>MIN($R$5:$R$10)</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>MAX($R$5:$R$10)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="O11:O13">
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>MIN($O$18:$O$23)</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>MAX($O$18:$O$23)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>